<commit_message>
Plantillas de anexos para informes de revisión
</commit_message>
<xml_diff>
--- a/plantillas/Anexo Comentarios Informe Revision Accesibilidad - Aplicaciones moviles.xlsx
+++ b/plantillas/Anexo Comentarios Informe Revision Accesibilidad - Aplicaciones moviles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseR\Mi unidad\curso2021-2022\accesibilidad Castellon\Temas\Taller\Plantillas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JoseR\Mi unidad\github\accesibilidad\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD8F061-0864-4EAC-9E69-FD5834A3BF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E431BB7-244E-4C87-A8CD-CEC1F004A705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Procesos" sheetId="45" r:id="rId1"/>
@@ -52,7 +52,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>La Decisión (UE) 2018/1524, en su apartado 3.3 indica que si cualquiera de las pantalla de la muestra seleccionada es una etapa de un proceso, deberán verificarse todas las etapas del proceso. Los procesos son posibles casos de uso de la aplicación móvil por parte de los usuarios.</t>
+          <t>La Decisión (UE) 2018/1524 indica que si cualquiera de las pantalla de la muestra seleccionada es una etapa de un proceso, deberán verificarse todas las etapas del proceso. Los procesos son posibles casos de uso de la aplicación móvil por parte de los usuarios.</t>
         </r>
       </text>
     </comment>
@@ -855,9 +855,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -866,6 +863,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
@@ -1161,79 +1161,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33" customHeight="1">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>188</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>99</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" s="1" customFormat="1">
-      <c r="A3" s="16"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" s="1" customFormat="1">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" s="1" customFormat="1">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="19" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" s="1" customFormat="1">
-      <c r="A7" s="16"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="2"/>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" s="1" customFormat="1">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="2"/>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" s="1" customFormat="1">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="2"/>
       <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" s="1" customFormat="1">
-      <c r="A10" s="16" t="s">
+      <c r="A10" s="19" t="s">
         <v>28</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="3"/>
     </row>
     <row r="11" spans="1:3" s="1" customFormat="1">
-      <c r="A11" s="16"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" s="1" customFormat="1">
-      <c r="A12" s="16"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:3" s="1" customFormat="1">
-      <c r="A13" s="16"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="2"/>
       <c r="C13" s="3"/>
     </row>
@@ -1363,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1410,10 +1410,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="39.6">
-      <c r="A2" s="17">
+      <c r="A2" s="16">
         <v>1</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="15"/>
@@ -1425,10 +1425,10 @@
       <c r="I2" s="14"/>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="17">
+      <c r="A3" s="16">
         <v>2</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="15"/>
@@ -1440,10 +1440,10 @@
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:9" ht="52.8">
-      <c r="A4" s="17">
+      <c r="A4" s="16">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="15"/>
@@ -1455,10 +1455,10 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:9" ht="26.4">
-      <c r="A5" s="17">
+      <c r="A5" s="16">
         <v>4</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>104</v>
       </c>
       <c r="C5" s="15"/>
@@ -1470,10 +1470,10 @@
       <c r="I5" s="14"/>
     </row>
     <row r="6" spans="1:9" ht="39.6">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>5</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C6" s="15"/>
@@ -1485,10 +1485,10 @@
       <c r="I6" s="14"/>
     </row>
     <row r="7" spans="1:9" ht="26.4">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>6</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>106</v>
       </c>
       <c r="C7" s="15"/>
@@ -1500,10 +1500,10 @@
       <c r="I7" s="14"/>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="17">
+      <c r="A8" s="16">
         <v>7</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>107</v>
       </c>
       <c r="C8" s="15"/>
@@ -1515,10 +1515,10 @@
       <c r="I8" s="14"/>
     </row>
     <row r="9" spans="1:9" ht="26.4">
-      <c r="A9" s="17">
+      <c r="A9" s="16">
         <v>8</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>108</v>
       </c>
       <c r="C9" s="15"/>
@@ -1530,10 +1530,10 @@
       <c r="I9" s="14"/>
     </row>
     <row r="10" spans="1:9" ht="26.4">
-      <c r="A10" s="17">
+      <c r="A10" s="16">
         <v>9</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>109</v>
       </c>
       <c r="C10" s="15"/>
@@ -1545,10 +1545,10 @@
       <c r="I10" s="14"/>
     </row>
     <row r="11" spans="1:9" ht="26.4">
-      <c r="A11" s="17">
+      <c r="A11" s="16">
         <v>10</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>110</v>
       </c>
       <c r="C11" s="15"/>
@@ -1560,10 +1560,10 @@
       <c r="I11" s="14"/>
     </row>
     <row r="12" spans="1:9" ht="26.4">
-      <c r="A12" s="17">
+      <c r="A12" s="16">
         <v>11</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="15"/>
@@ -1575,10 +1575,10 @@
       <c r="I12" s="14"/>
     </row>
     <row r="13" spans="1:9" ht="26.4">
-      <c r="A13" s="17">
+      <c r="A13" s="16">
         <v>12</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="15"/>
@@ -1590,10 +1590,10 @@
       <c r="I13" s="14"/>
     </row>
     <row r="14" spans="1:9" ht="26.4">
-      <c r="A14" s="17">
+      <c r="A14" s="16">
         <v>13</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="16" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="15"/>
@@ -1605,10 +1605,10 @@
       <c r="I14" s="14"/>
     </row>
     <row r="15" spans="1:9" ht="39.6">
-      <c r="A15" s="17">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="16" t="s">
         <v>111</v>
       </c>
       <c r="C15" s="15"/>
@@ -1620,10 +1620,10 @@
       <c r="I15" s="14"/>
     </row>
     <row r="16" spans="1:9" ht="52.8">
-      <c r="A16" s="17">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="16" t="s">
         <v>32</v>
       </c>
       <c r="C16" s="15"/>
@@ -1635,10 +1635,10 @@
       <c r="I16" s="14"/>
     </row>
     <row r="17" spans="1:9" ht="26.4">
-      <c r="A17" s="17">
+      <c r="A17" s="16">
         <v>16</v>
       </c>
-      <c r="B17" s="18" t="s">
+      <c r="B17" s="17" t="s">
         <v>81</v>
       </c>
       <c r="C17" s="15"/>
@@ -1650,10 +1650,10 @@
       <c r="I17" s="14"/>
     </row>
     <row r="18" spans="1:9" ht="26.4">
-      <c r="A18" s="17">
+      <c r="A18" s="16">
         <v>17</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="17" t="s">
         <v>82</v>
       </c>
       <c r="C18" s="15"/>
@@ -1665,10 +1665,10 @@
       <c r="I18" s="14"/>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="17">
+      <c r="A19" s="16">
         <v>18</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="B19" s="17" t="s">
         <v>83</v>
       </c>
       <c r="C19" s="15"/>
@@ -1680,10 +1680,10 @@
       <c r="I19" s="14"/>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="17">
+      <c r="A20" s="16">
         <v>19</v>
       </c>
-      <c r="B20" s="18" t="s">
+      <c r="B20" s="17" t="s">
         <v>84</v>
       </c>
       <c r="C20" s="15"/>
@@ -1695,10 +1695,10 @@
       <c r="I20" s="14"/>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="17">
+      <c r="A21" s="16">
         <v>20</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="17" t="s">
         <v>85</v>
       </c>
       <c r="C21" s="15"/>
@@ -1710,10 +1710,10 @@
       <c r="I21" s="14"/>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="17">
+      <c r="A22" s="16">
         <v>21</v>
       </c>
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C22" s="15"/>
@@ -1725,10 +1725,10 @@
       <c r="I22" s="14"/>
     </row>
     <row r="23" spans="1:9" ht="39.6">
-      <c r="A23" s="17">
+      <c r="A23" s="16">
         <v>22</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="16" t="s">
         <v>112</v>
       </c>
       <c r="C23" s="15"/>
@@ -1740,10 +1740,10 @@
       <c r="I23" s="14"/>
     </row>
     <row r="24" spans="1:9" ht="26.4">
-      <c r="A24" s="17">
+      <c r="A24" s="16">
         <v>23</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C24" s="15"/>
@@ -1755,10 +1755,10 @@
       <c r="I24" s="14"/>
     </row>
     <row r="25" spans="1:9" ht="26.4">
-      <c r="A25" s="17">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="16" t="s">
         <v>33</v>
       </c>
       <c r="C25" s="15"/>
@@ -1770,10 +1770,10 @@
       <c r="I25" s="14"/>
     </row>
     <row r="26" spans="1:9">
-      <c r="A26" s="17">
+      <c r="A26" s="16">
         <v>25</v>
       </c>
-      <c r="B26" s="17" t="s">
+      <c r="B26" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C26" s="15"/>
@@ -1785,10 +1785,10 @@
       <c r="I26" s="14"/>
     </row>
     <row r="27" spans="1:9" ht="26.4">
-      <c r="A27" s="17">
+      <c r="A27" s="16">
         <v>26</v>
       </c>
-      <c r="B27" s="17" t="s">
+      <c r="B27" s="16" t="s">
         <v>6</v>
       </c>
       <c r="C27" s="15"/>
@@ -1800,10 +1800,10 @@
       <c r="I27" s="14"/>
     </row>
     <row r="28" spans="1:9" ht="26.4">
-      <c r="A28" s="17">
+      <c r="A28" s="16">
         <v>27</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B28" s="16" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="15"/>
@@ -1815,7 +1815,7 @@
       <c r="I28" s="14"/>
     </row>
     <row r="29" spans="1:9" ht="26.4">
-      <c r="A29" s="17">
+      <c r="A29" s="16">
         <v>28</v>
       </c>
       <c r="B29" s="11" t="s">
@@ -1830,7 +1830,7 @@
       <c r="I29" s="14"/>
     </row>
     <row r="30" spans="1:9" ht="52.8">
-      <c r="A30" s="17">
+      <c r="A30" s="16">
         <v>29</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -1845,10 +1845,10 @@
       <c r="I30" s="14"/>
     </row>
     <row r="31" spans="1:9" ht="26.4">
-      <c r="A31" s="17">
+      <c r="A31" s="16">
         <v>30</v>
       </c>
-      <c r="B31" s="17" t="s">
+      <c r="B31" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C31" s="15"/>
@@ -1860,10 +1860,10 @@
       <c r="I31" s="14"/>
     </row>
     <row r="32" spans="1:9" ht="26.4">
-      <c r="A32" s="17">
+      <c r="A32" s="16">
         <v>31</v>
       </c>
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="16" t="s">
         <v>8</v>
       </c>
       <c r="C32" s="15"/>
@@ -1875,10 +1875,10 @@
       <c r="I32" s="14"/>
     </row>
     <row r="33" spans="1:9" ht="26.4">
-      <c r="A33" s="17">
+      <c r="A33" s="16">
         <v>32</v>
       </c>
-      <c r="B33" s="17" t="s">
+      <c r="B33" s="16" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="15"/>
@@ -1890,7 +1890,7 @@
       <c r="I33" s="14"/>
     </row>
     <row r="34" spans="1:9" ht="26.4">
-      <c r="A34" s="17">
+      <c r="A34" s="16">
         <v>33</v>
       </c>
       <c r="B34" s="11" t="s">
@@ -1905,7 +1905,7 @@
       <c r="I34" s="14"/>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="17">
+      <c r="A35" s="16">
         <v>34</v>
       </c>
       <c r="B35" s="11" t="s">
@@ -1920,10 +1920,10 @@
       <c r="I35" s="14"/>
     </row>
     <row r="36" spans="1:9" ht="26.4">
-      <c r="A36" s="17">
+      <c r="A36" s="16">
         <v>35</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C36" s="15"/>
@@ -1935,10 +1935,10 @@
       <c r="I36" s="14"/>
     </row>
     <row r="37" spans="1:9" ht="26.4">
-      <c r="A37" s="17">
+      <c r="A37" s="16">
         <v>36</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>11</v>
       </c>
       <c r="C37" s="15"/>
@@ -1950,10 +1950,10 @@
       <c r="I37" s="14"/>
     </row>
     <row r="38" spans="1:9" ht="26.4">
-      <c r="A38" s="17">
+      <c r="A38" s="16">
         <v>37</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C38" s="15"/>
@@ -1965,10 +1965,10 @@
       <c r="I38" s="14"/>
     </row>
     <row r="39" spans="1:9" ht="39.6">
-      <c r="A39" s="17">
+      <c r="A39" s="16">
         <v>38</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="15"/>
@@ -1980,10 +1980,10 @@
       <c r="I39" s="14"/>
     </row>
     <row r="40" spans="1:9" ht="26.4">
-      <c r="A40" s="17">
+      <c r="A40" s="16">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>35</v>
       </c>
       <c r="C40" s="15"/>
@@ -1995,10 +1995,10 @@
       <c r="I40" s="14"/>
     </row>
     <row r="41" spans="1:9" ht="26.4">
-      <c r="A41" s="17">
+      <c r="A41" s="16">
         <v>40</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>36</v>
       </c>
       <c r="C41" s="15"/>
@@ -2010,10 +2010,10 @@
       <c r="I41" s="14"/>
     </row>
     <row r="42" spans="1:9" ht="26.4">
-      <c r="A42" s="17">
+      <c r="A42" s="16">
         <v>41</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>38</v>
       </c>
       <c r="C42" s="15"/>
@@ -2025,10 +2025,10 @@
       <c r="I42" s="14"/>
     </row>
     <row r="43" spans="1:9" ht="52.8">
-      <c r="A43" s="17">
+      <c r="A43" s="16">
         <v>42</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C43" s="15"/>
@@ -2040,10 +2040,10 @@
       <c r="I43" s="14"/>
     </row>
     <row r="44" spans="1:9" ht="39.6">
-      <c r="A44" s="17">
+      <c r="A44" s="16">
         <v>43</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>39</v>
       </c>
       <c r="C44" s="15"/>
@@ -2055,10 +2055,10 @@
       <c r="I44" s="14"/>
     </row>
     <row r="45" spans="1:9" ht="26.4">
-      <c r="A45" s="17">
+      <c r="A45" s="16">
         <v>44</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>40</v>
       </c>
       <c r="C45" s="15"/>
@@ -2070,10 +2070,10 @@
       <c r="I45" s="14"/>
     </row>
     <row r="46" spans="1:9" ht="26.4">
-      <c r="A46" s="17">
+      <c r="A46" s="16">
         <v>45</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>41</v>
       </c>
       <c r="C46" s="15"/>
@@ -2085,10 +2085,10 @@
       <c r="I46" s="14"/>
     </row>
     <row r="47" spans="1:9" ht="26.4">
-      <c r="A47" s="17">
+      <c r="A47" s="16">
         <v>46</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>42</v>
       </c>
       <c r="C47" s="15"/>
@@ -2100,10 +2100,10 @@
       <c r="I47" s="14"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="17">
+      <c r="A48" s="16">
         <v>47</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>43</v>
       </c>
       <c r="C48" s="15"/>
@@ -2115,10 +2115,10 @@
       <c r="I48" s="14"/>
     </row>
     <row r="49" spans="1:9" ht="39.6">
-      <c r="A49" s="17">
+      <c r="A49" s="16">
         <v>48</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>44</v>
       </c>
       <c r="C49" s="15"/>
@@ -2130,10 +2130,10 @@
       <c r="I49" s="14"/>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="17">
+      <c r="A50" s="16">
         <v>49</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C50" s="15"/>
@@ -2145,10 +2145,10 @@
       <c r="I50" s="14"/>
     </row>
     <row r="51" spans="1:9" ht="26.4">
-      <c r="A51" s="17">
+      <c r="A51" s="16">
         <v>50</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="16" t="s">
         <v>46</v>
       </c>
       <c r="C51" s="15"/>
@@ -2160,10 +2160,10 @@
       <c r="I51" s="14"/>
     </row>
     <row r="52" spans="1:9" ht="26.4">
-      <c r="A52" s="17">
+      <c r="A52" s="16">
         <v>51</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="16" t="s">
         <v>47</v>
       </c>
       <c r="C52" s="15"/>
@@ -2175,10 +2175,10 @@
       <c r="I52" s="14"/>
     </row>
     <row r="53" spans="1:9" ht="26.4">
-      <c r="A53" s="17">
+      <c r="A53" s="16">
         <v>52</v>
       </c>
-      <c r="B53" s="17" t="s">
+      <c r="B53" s="16" t="s">
         <v>48</v>
       </c>
       <c r="C53" s="15"/>
@@ -2190,10 +2190,10 @@
       <c r="I53" s="14"/>
     </row>
     <row r="54" spans="1:9" ht="26.4">
-      <c r="A54" s="17">
+      <c r="A54" s="16">
         <v>53</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="16" t="s">
         <v>49</v>
       </c>
       <c r="C54" s="15"/>
@@ -2205,10 +2205,10 @@
       <c r="I54" s="14"/>
     </row>
     <row r="55" spans="1:9" ht="26.4">
-      <c r="A55" s="17">
+      <c r="A55" s="16">
         <v>54</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="16" t="s">
         <v>50</v>
       </c>
       <c r="C55" s="15"/>
@@ -2220,10 +2220,10 @@
       <c r="I55" s="14"/>
     </row>
     <row r="56" spans="1:9" ht="26.4">
-      <c r="A56" s="17">
+      <c r="A56" s="16">
         <v>55</v>
       </c>
-      <c r="B56" s="17" t="s">
+      <c r="B56" s="16" t="s">
         <v>51</v>
       </c>
       <c r="C56" s="15"/>
@@ -2235,10 +2235,10 @@
       <c r="I56" s="14"/>
     </row>
     <row r="57" spans="1:9" ht="26.4">
-      <c r="A57" s="17">
+      <c r="A57" s="16">
         <v>56</v>
       </c>
-      <c r="B57" s="17" t="s">
+      <c r="B57" s="16" t="s">
         <v>52</v>
       </c>
       <c r="C57" s="15"/>
@@ -2250,10 +2250,10 @@
       <c r="I57" s="14"/>
     </row>
     <row r="58" spans="1:9" ht="39.6">
-      <c r="A58" s="17">
+      <c r="A58" s="16">
         <v>57</v>
       </c>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="16" t="s">
         <v>53</v>
       </c>
       <c r="C58" s="15"/>
@@ -2265,10 +2265,10 @@
       <c r="I58" s="14"/>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="17">
+      <c r="A59" s="16">
         <v>58</v>
       </c>
-      <c r="B59" s="17" t="s">
+      <c r="B59" s="16" t="s">
         <v>54</v>
       </c>
       <c r="C59" s="15"/>
@@ -2280,10 +2280,10 @@
       <c r="I59" s="14"/>
     </row>
     <row r="60" spans="1:9" ht="26.4">
-      <c r="A60" s="17">
+      <c r="A60" s="16">
         <v>59</v>
       </c>
-      <c r="B60" s="17" t="s">
+      <c r="B60" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C60" s="15"/>
@@ -2295,10 +2295,10 @@
       <c r="I60" s="14"/>
     </row>
     <row r="61" spans="1:9" ht="26.4">
-      <c r="A61" s="17">
+      <c r="A61" s="16">
         <v>60</v>
       </c>
-      <c r="B61" s="17" t="s">
+      <c r="B61" s="16" t="s">
         <v>56</v>
       </c>
       <c r="C61" s="15"/>
@@ -2310,10 +2310,10 @@
       <c r="I61" s="14"/>
     </row>
     <row r="62" spans="1:9" ht="26.4">
-      <c r="A62" s="17">
+      <c r="A62" s="16">
         <v>61</v>
       </c>
-      <c r="B62" s="17" t="s">
+      <c r="B62" s="16" t="s">
         <v>57</v>
       </c>
       <c r="C62" s="15"/>
@@ -2325,10 +2325,10 @@
       <c r="I62" s="14"/>
     </row>
     <row r="63" spans="1:9" ht="26.4">
-      <c r="A63" s="17">
+      <c r="A63" s="16">
         <v>62</v>
       </c>
-      <c r="B63" s="17" t="s">
+      <c r="B63" s="16" t="s">
         <v>58</v>
       </c>
       <c r="C63" s="15"/>
@@ -2340,10 +2340,10 @@
       <c r="I63" s="14"/>
     </row>
     <row r="64" spans="1:9" ht="26.4">
-      <c r="A64" s="17">
+      <c r="A64" s="16">
         <v>63</v>
       </c>
-      <c r="B64" s="17" t="s">
+      <c r="B64" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="15"/>
@@ -2355,10 +2355,10 @@
       <c r="I64" s="14"/>
     </row>
     <row r="65" spans="1:9" ht="26.4">
-      <c r="A65" s="17">
+      <c r="A65" s="16">
         <v>64</v>
       </c>
-      <c r="B65" s="17" t="s">
+      <c r="B65" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="15"/>
@@ -2370,10 +2370,10 @@
       <c r="I65" s="14"/>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="17">
+      <c r="A66" s="16">
         <v>65</v>
       </c>
-      <c r="B66" s="17" t="s">
+      <c r="B66" s="16" t="s">
         <v>60</v>
       </c>
       <c r="C66" s="15"/>
@@ -2385,10 +2385,10 @@
       <c r="I66" s="14"/>
     </row>
     <row r="67" spans="1:9" ht="26.4">
-      <c r="A67" s="17">
+      <c r="A67" s="16">
         <v>66</v>
       </c>
-      <c r="B67" s="17" t="s">
+      <c r="B67" s="16" t="s">
         <v>61</v>
       </c>
       <c r="C67" s="15"/>
@@ -2400,10 +2400,10 @@
       <c r="I67" s="14"/>
     </row>
     <row r="68" spans="1:9" ht="26.4">
-      <c r="A68" s="17">
+      <c r="A68" s="16">
         <v>67</v>
       </c>
-      <c r="B68" s="17" t="s">
+      <c r="B68" s="16" t="s">
         <v>62</v>
       </c>
       <c r="C68" s="15"/>
@@ -2415,10 +2415,10 @@
       <c r="I68" s="14"/>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="17">
+      <c r="A69" s="16">
         <v>68</v>
       </c>
-      <c r="B69" s="17" t="s">
+      <c r="B69" s="16" t="s">
         <v>63</v>
       </c>
       <c r="C69" s="15"/>
@@ -2430,10 +2430,10 @@
       <c r="I69" s="14"/>
     </row>
     <row r="70" spans="1:9" ht="26.4">
-      <c r="A70" s="17">
+      <c r="A70" s="16">
         <v>69</v>
       </c>
-      <c r="B70" s="17" t="s">
+      <c r="B70" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C70" s="15"/>
@@ -2445,10 +2445,10 @@
       <c r="I70" s="14"/>
     </row>
     <row r="71" spans="1:9" ht="26.4">
-      <c r="A71" s="17">
+      <c r="A71" s="16">
         <v>70</v>
       </c>
-      <c r="B71" s="17" t="s">
+      <c r="B71" s="16" t="s">
         <v>65</v>
       </c>
       <c r="C71" s="15"/>
@@ -2460,10 +2460,10 @@
       <c r="I71" s="14"/>
     </row>
     <row r="72" spans="1:9" ht="26.4">
-      <c r="A72" s="17">
+      <c r="A72" s="16">
         <v>71</v>
       </c>
-      <c r="B72" s="17" t="s">
+      <c r="B72" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C72" s="15"/>
@@ -2475,10 +2475,10 @@
       <c r="I72" s="14"/>
     </row>
     <row r="73" spans="1:9" ht="26.4">
-      <c r="A73" s="17">
+      <c r="A73" s="16">
         <v>72</v>
       </c>
-      <c r="B73" s="17" t="s">
+      <c r="B73" s="16" t="s">
         <v>67</v>
       </c>
       <c r="C73" s="15"/>
@@ -2490,10 +2490,10 @@
       <c r="I73" s="14"/>
     </row>
     <row r="74" spans="1:9" ht="26.4">
-      <c r="A74" s="17">
+      <c r="A74" s="16">
         <v>73</v>
       </c>
-      <c r="B74" s="17" t="s">
+      <c r="B74" s="16" t="s">
         <v>113</v>
       </c>
       <c r="C74" s="15"/>
@@ -2505,10 +2505,10 @@
       <c r="I74" s="14"/>
     </row>
     <row r="75" spans="1:9" ht="26.4">
-      <c r="A75" s="17">
+      <c r="A75" s="16">
         <v>74</v>
       </c>
-      <c r="B75" s="17" t="s">
+      <c r="B75" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C75" s="15"/>
@@ -2520,10 +2520,10 @@
       <c r="I75" s="14"/>
     </row>
     <row r="76" spans="1:9" ht="26.4">
-      <c r="A76" s="17">
+      <c r="A76" s="16">
         <v>75</v>
       </c>
-      <c r="B76" s="17" t="s">
+      <c r="B76" s="16" t="s">
         <v>68</v>
       </c>
       <c r="C76" s="15"/>
@@ -2535,10 +2535,10 @@
       <c r="I76" s="14"/>
     </row>
     <row r="77" spans="1:9" ht="26.4">
-      <c r="A77" s="17">
+      <c r="A77" s="16">
         <v>76</v>
       </c>
-      <c r="B77" s="17" t="s">
+      <c r="B77" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C77" s="15"/>
@@ -2550,10 +2550,10 @@
       <c r="I77" s="14"/>
     </row>
     <row r="78" spans="1:9" ht="26.4">
-      <c r="A78" s="17">
+      <c r="A78" s="16">
         <v>77</v>
       </c>
-      <c r="B78" s="17" t="s">
+      <c r="B78" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C78" s="15"/>
@@ -2565,10 +2565,10 @@
       <c r="I78" s="14"/>
     </row>
     <row r="79" spans="1:9" ht="26.4">
-      <c r="A79" s="17">
+      <c r="A79" s="16">
         <v>78</v>
       </c>
-      <c r="B79" s="17" t="s">
+      <c r="B79" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C79" s="15"/>
@@ -2580,10 +2580,10 @@
       <c r="I79" s="14"/>
     </row>
     <row r="80" spans="1:9" ht="26.4">
-      <c r="A80" s="17">
+      <c r="A80" s="16">
         <v>79</v>
       </c>
-      <c r="B80" s="17" t="s">
+      <c r="B80" s="16" t="s">
         <v>72</v>
       </c>
       <c r="C80" s="15"/>
@@ -2595,10 +2595,10 @@
       <c r="I80" s="14"/>
     </row>
     <row r="81" spans="1:9" ht="39.6">
-      <c r="A81" s="17">
+      <c r="A81" s="16">
         <v>80</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C81" s="15"/>
@@ -2610,10 +2610,10 @@
       <c r="I81" s="14"/>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="17">
+      <c r="A82" s="16">
         <v>81</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="16" t="s">
         <v>76</v>
       </c>
       <c r="C82" s="15"/>
@@ -2625,10 +2625,10 @@
       <c r="I82" s="14"/>
     </row>
     <row r="83" spans="1:9" ht="26.4">
-      <c r="A83" s="17">
+      <c r="A83" s="16">
         <v>82</v>
       </c>
-      <c r="B83" s="17" t="s">
+      <c r="B83" s="16" t="s">
         <v>74</v>
       </c>
       <c r="C83" s="15"/>
@@ -2640,10 +2640,10 @@
       <c r="I83" s="14"/>
     </row>
     <row r="84" spans="1:9" ht="26.4">
-      <c r="A84" s="17">
+      <c r="A84" s="16">
         <v>83</v>
       </c>
-      <c r="B84" s="17" t="s">
+      <c r="B84" s="16" t="s">
         <v>75</v>
       </c>
       <c r="C84" s="15"/>
@@ -2655,10 +2655,10 @@
       <c r="I84" s="14"/>
     </row>
     <row r="85" spans="1:9" ht="39.6">
-      <c r="A85" s="17">
+      <c r="A85" s="16">
         <v>84</v>
       </c>
-      <c r="B85" s="17" t="s">
+      <c r="B85" s="16" t="s">
         <v>114</v>
       </c>
       <c r="C85" s="15"/>
@@ -2670,10 +2670,10 @@
       <c r="I85" s="14"/>
     </row>
     <row r="86" spans="1:9" ht="39.6">
-      <c r="A86" s="17">
+      <c r="A86" s="16">
         <v>85</v>
       </c>
-      <c r="B86" s="17" t="s">
+      <c r="B86" s="16" t="s">
         <v>115</v>
       </c>
       <c r="C86" s="15"/>
@@ -2685,10 +2685,10 @@
       <c r="I86" s="14"/>
     </row>
     <row r="87" spans="1:9" ht="39.6">
-      <c r="A87" s="17">
+      <c r="A87" s="16">
         <v>86</v>
       </c>
-      <c r="B87" s="17" t="s">
+      <c r="B87" s="16" t="s">
         <v>116</v>
       </c>
       <c r="C87" s="15"/>
@@ -2700,10 +2700,10 @@
       <c r="I87" s="14"/>
     </row>
     <row r="88" spans="1:9" ht="39.6">
-      <c r="A88" s="17">
+      <c r="A88" s="16">
         <v>87</v>
       </c>
-      <c r="B88" s="17" t="s">
+      <c r="B88" s="16" t="s">
         <v>117</v>
       </c>
       <c r="C88" s="15"/>
@@ -2715,10 +2715,10 @@
       <c r="I88" s="14"/>
     </row>
     <row r="89" spans="1:9" ht="26.4">
-      <c r="A89" s="17">
+      <c r="A89" s="16">
         <v>88</v>
       </c>
-      <c r="B89" s="17" t="s">
+      <c r="B89" s="16" t="s">
         <v>118</v>
       </c>
       <c r="C89" s="15"/>
@@ -2730,10 +2730,10 @@
       <c r="I89" s="14"/>
     </row>
     <row r="90" spans="1:9" ht="66">
-      <c r="A90" s="17">
+      <c r="A90" s="16">
         <v>89</v>
       </c>
-      <c r="B90" s="17" t="s">
+      <c r="B90" s="16" t="s">
         <v>119</v>
       </c>
       <c r="C90" s="15"/>
@@ -2745,10 +2745,10 @@
       <c r="I90" s="14"/>
     </row>
     <row r="91" spans="1:9" ht="66">
-      <c r="A91" s="17">
+      <c r="A91" s="16">
         <v>90</v>
       </c>
-      <c r="B91" s="17" t="s">
+      <c r="B91" s="16" t="s">
         <v>120</v>
       </c>
       <c r="C91" s="15"/>
@@ -2760,10 +2760,10 @@
       <c r="I91" s="14"/>
     </row>
     <row r="92" spans="1:9" ht="39.6">
-      <c r="A92" s="17">
+      <c r="A92" s="16">
         <v>91</v>
       </c>
-      <c r="B92" s="17" t="s">
+      <c r="B92" s="16" t="s">
         <v>121</v>
       </c>
       <c r="C92" s="15"/>
@@ -2775,10 +2775,10 @@
       <c r="I92" s="14"/>
     </row>
     <row r="93" spans="1:9" ht="39.6">
-      <c r="A93" s="17">
+      <c r="A93" s="16">
         <v>92</v>
       </c>
-      <c r="B93" s="17" t="s">
+      <c r="B93" s="16" t="s">
         <v>122</v>
       </c>
       <c r="C93" s="15"/>
@@ -2790,10 +2790,10 @@
       <c r="I93" s="14"/>
     </row>
     <row r="94" spans="1:9" ht="39.6">
-      <c r="A94" s="17">
+      <c r="A94" s="16">
         <v>93</v>
       </c>
-      <c r="B94" s="17" t="s">
+      <c r="B94" s="16" t="s">
         <v>123</v>
       </c>
       <c r="C94" s="15"/>
@@ -2805,10 +2805,10 @@
       <c r="I94" s="14"/>
     </row>
     <row r="95" spans="1:9" ht="26.4">
-      <c r="A95" s="17">
+      <c r="A95" s="16">
         <v>94</v>
       </c>
-      <c r="B95" s="17" t="s">
+      <c r="B95" s="16" t="s">
         <v>124</v>
       </c>
       <c r="C95" s="15"/>
@@ -2820,10 +2820,10 @@
       <c r="I95" s="14"/>
     </row>
     <row r="96" spans="1:9">
-      <c r="A96" s="17">
+      <c r="A96" s="16">
         <v>95</v>
       </c>
-      <c r="B96" s="17" t="s">
+      <c r="B96" s="16" t="s">
         <v>125</v>
       </c>
       <c r="C96" s="15"/>
@@ -2835,10 +2835,10 @@
       <c r="I96" s="14"/>
     </row>
     <row r="97" spans="1:9" ht="52.8">
-      <c r="A97" s="17">
+      <c r="A97" s="16">
         <v>96</v>
       </c>
-      <c r="B97" s="17" t="s">
+      <c r="B97" s="16" t="s">
         <v>126</v>
       </c>
       <c r="C97" s="15"/>
@@ -2850,10 +2850,10 @@
       <c r="I97" s="14"/>
     </row>
     <row r="98" spans="1:9" ht="52.8">
-      <c r="A98" s="17">
+      <c r="A98" s="16">
         <v>97</v>
       </c>
-      <c r="B98" s="17" t="s">
+      <c r="B98" s="16" t="s">
         <v>127</v>
       </c>
       <c r="C98" s="15"/>
@@ -2865,10 +2865,10 @@
       <c r="I98" s="14"/>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="17">
+      <c r="A99" s="16">
         <v>98</v>
       </c>
-      <c r="B99" s="17" t="s">
+      <c r="B99" s="16" t="s">
         <v>128</v>
       </c>
       <c r="C99" s="15"/>
@@ -2880,10 +2880,10 @@
       <c r="I99" s="14"/>
     </row>
     <row r="100" spans="1:9" ht="26.4">
-      <c r="A100" s="17">
+      <c r="A100" s="16">
         <v>99</v>
       </c>
-      <c r="B100" s="17" t="s">
+      <c r="B100" s="16" t="s">
         <v>129</v>
       </c>
       <c r="C100" s="15"/>
@@ -2895,10 +2895,10 @@
       <c r="I100" s="14"/>
     </row>
     <row r="101" spans="1:9" ht="26.4">
-      <c r="A101" s="17">
+      <c r="A101" s="16">
         <v>100</v>
       </c>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="16" t="s">
         <v>130</v>
       </c>
       <c r="C101" s="15"/>
@@ -2910,10 +2910,10 @@
       <c r="I101" s="14"/>
     </row>
     <row r="102" spans="1:9" ht="39.6">
-      <c r="A102" s="17">
+      <c r="A102" s="16">
         <v>101</v>
       </c>
-      <c r="B102" s="17" t="s">
+      <c r="B102" s="16" t="s">
         <v>131</v>
       </c>
       <c r="C102" s="15"/>
@@ -2925,10 +2925,10 @@
       <c r="I102" s="14"/>
     </row>
     <row r="103" spans="1:9" ht="39.6">
-      <c r="A103" s="17">
+      <c r="A103" s="16">
         <v>102</v>
       </c>
-      <c r="B103" s="17" t="s">
+      <c r="B103" s="16" t="s">
         <v>132</v>
       </c>
       <c r="C103" s="15"/>
@@ -2940,10 +2940,10 @@
       <c r="I103" s="14"/>
     </row>
     <row r="104" spans="1:9" ht="39.6">
-      <c r="A104" s="17">
+      <c r="A104" s="16">
         <v>103</v>
       </c>
-      <c r="B104" s="17" t="s">
+      <c r="B104" s="16" t="s">
         <v>133</v>
       </c>
       <c r="C104" s="15"/>
@@ -2955,7 +2955,7 @@
       <c r="I104" s="14"/>
     </row>
     <row r="105" spans="1:9" ht="39.6">
-      <c r="A105" s="17">
+      <c r="A105" s="16">
         <v>104</v>
       </c>
       <c r="B105" s="11" t="s">
@@ -2970,10 +2970,10 @@
       <c r="I105" s="14"/>
     </row>
     <row r="106" spans="1:9" ht="26.4">
-      <c r="A106" s="17">
+      <c r="A106" s="16">
         <v>105</v>
       </c>
-      <c r="B106" s="17" t="s">
+      <c r="B106" s="16" t="s">
         <v>135</v>
       </c>
       <c r="C106" s="15"/>
@@ -2985,10 +2985,10 @@
       <c r="I106" s="14"/>
     </row>
     <row r="107" spans="1:9" ht="26.4">
-      <c r="A107" s="17">
+      <c r="A107" s="16">
         <v>106</v>
       </c>
-      <c r="B107" s="17" t="s">
+      <c r="B107" s="16" t="s">
         <v>136</v>
       </c>
       <c r="C107" s="15"/>
@@ -3000,10 +3000,10 @@
       <c r="I107" s="14"/>
     </row>
     <row r="108" spans="1:9" ht="26.4">
-      <c r="A108" s="17">
+      <c r="A108" s="16">
         <v>107</v>
       </c>
-      <c r="B108" s="17" t="s">
+      <c r="B108" s="16" t="s">
         <v>137</v>
       </c>
       <c r="C108" s="15"/>
@@ -3015,10 +3015,10 @@
       <c r="I108" s="14"/>
     </row>
     <row r="109" spans="1:9" ht="39.6">
-      <c r="A109" s="17">
+      <c r="A109" s="16">
         <v>108</v>
       </c>
-      <c r="B109" s="17" t="s">
+      <c r="B109" s="16" t="s">
         <v>138</v>
       </c>
       <c r="C109" s="15"/>
@@ -3030,10 +3030,10 @@
       <c r="I109" s="14"/>
     </row>
     <row r="110" spans="1:9" ht="26.4">
-      <c r="A110" s="17">
+      <c r="A110" s="16">
         <v>109</v>
       </c>
-      <c r="B110" s="17" t="s">
+      <c r="B110" s="16" t="s">
         <v>139</v>
       </c>
       <c r="C110" s="15"/>
@@ -3045,10 +3045,10 @@
       <c r="I110" s="14"/>
     </row>
     <row r="111" spans="1:9" ht="26.4">
-      <c r="A111" s="17">
+      <c r="A111" s="16">
         <v>110</v>
       </c>
-      <c r="B111" s="17" t="s">
+      <c r="B111" s="16" t="s">
         <v>140</v>
       </c>
       <c r="C111" s="15"/>
@@ -3060,10 +3060,10 @@
       <c r="I111" s="14"/>
     </row>
     <row r="112" spans="1:9" ht="26.4">
-      <c r="A112" s="17">
+      <c r="A112" s="16">
         <v>111</v>
       </c>
-      <c r="B112" s="17" t="s">
+      <c r="B112" s="16" t="s">
         <v>141</v>
       </c>
       <c r="C112" s="15"/>
@@ -3075,10 +3075,10 @@
       <c r="I112" s="14"/>
     </row>
     <row r="113" spans="1:9" ht="39.6">
-      <c r="A113" s="17">
+      <c r="A113" s="16">
         <v>112</v>
       </c>
-      <c r="B113" s="17" t="s">
+      <c r="B113" s="16" t="s">
         <v>142</v>
       </c>
       <c r="C113" s="15"/>
@@ -3090,10 +3090,10 @@
       <c r="I113" s="14"/>
     </row>
     <row r="114" spans="1:9" ht="39.6">
-      <c r="A114" s="17">
+      <c r="A114" s="16">
         <v>113</v>
       </c>
-      <c r="B114" s="17" t="s">
+      <c r="B114" s="16" t="s">
         <v>143</v>
       </c>
       <c r="C114" s="15"/>
@@ -3105,10 +3105,10 @@
       <c r="I114" s="14"/>
     </row>
     <row r="115" spans="1:9" ht="26.4">
-      <c r="A115" s="17">
+      <c r="A115" s="16">
         <v>114</v>
       </c>
-      <c r="B115" s="17" t="s">
+      <c r="B115" s="16" t="s">
         <v>144</v>
       </c>
       <c r="C115" s="15"/>
@@ -3120,10 +3120,10 @@
       <c r="I115" s="14"/>
     </row>
     <row r="116" spans="1:9" ht="26.4">
-      <c r="A116" s="17">
+      <c r="A116" s="16">
         <v>115</v>
       </c>
-      <c r="B116" s="17" t="s">
+      <c r="B116" s="16" t="s">
         <v>145</v>
       </c>
       <c r="C116" s="15"/>
@@ -3135,10 +3135,10 @@
       <c r="I116" s="14"/>
     </row>
     <row r="117" spans="1:9" ht="26.4">
-      <c r="A117" s="17">
+      <c r="A117" s="16">
         <v>116</v>
       </c>
-      <c r="B117" s="17" t="s">
+      <c r="B117" s="16" t="s">
         <v>146</v>
       </c>
       <c r="C117" s="15"/>
@@ -3150,10 +3150,10 @@
       <c r="I117" s="14"/>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="17">
+      <c r="A118" s="16">
         <v>117</v>
       </c>
-      <c r="B118" s="17" t="s">
+      <c r="B118" s="16" t="s">
         <v>147</v>
       </c>
       <c r="C118" s="15"/>
@@ -3165,10 +3165,10 @@
       <c r="I118" s="14"/>
     </row>
     <row r="119" spans="1:9" ht="26.4">
-      <c r="A119" s="17">
+      <c r="A119" s="16">
         <v>118</v>
       </c>
-      <c r="B119" s="17" t="s">
+      <c r="B119" s="16" t="s">
         <v>148</v>
       </c>
       <c r="C119" s="15"/>
@@ -3180,10 +3180,10 @@
       <c r="I119" s="14"/>
     </row>
     <row r="120" spans="1:9" ht="26.4">
-      <c r="A120" s="17">
+      <c r="A120" s="16">
         <v>119</v>
       </c>
-      <c r="B120" s="17" t="s">
+      <c r="B120" s="16" t="s">
         <v>149</v>
       </c>
       <c r="C120" s="15"/>
@@ -3195,10 +3195,10 @@
       <c r="I120" s="14"/>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="17">
+      <c r="A121" s="16">
         <v>120</v>
       </c>
-      <c r="B121" s="17" t="s">
+      <c r="B121" s="16" t="s">
         <v>150</v>
       </c>
       <c r="C121" s="15"/>
@@ -3210,10 +3210,10 @@
       <c r="I121" s="14"/>
     </row>
     <row r="122" spans="1:9" ht="26.4">
-      <c r="A122" s="17">
+      <c r="A122" s="16">
         <v>121</v>
       </c>
-      <c r="B122" s="17" t="s">
+      <c r="B122" s="16" t="s">
         <v>151</v>
       </c>
       <c r="C122" s="15"/>
@@ -3225,10 +3225,10 @@
       <c r="I122" s="14"/>
     </row>
     <row r="123" spans="1:9" ht="26.4">
-      <c r="A123" s="17">
+      <c r="A123" s="16">
         <v>122</v>
       </c>
-      <c r="B123" s="17" t="s">
+      <c r="B123" s="16" t="s">
         <v>152</v>
       </c>
       <c r="C123" s="15"/>
@@ -3240,10 +3240,10 @@
       <c r="I123" s="14"/>
     </row>
     <row r="124" spans="1:9" ht="39.6">
-      <c r="A124" s="17">
+      <c r="A124" s="16">
         <v>123</v>
       </c>
-      <c r="B124" s="17" t="s">
+      <c r="B124" s="16" t="s">
         <v>153</v>
       </c>
       <c r="C124" s="15"/>
@@ -3255,10 +3255,10 @@
       <c r="I124" s="14"/>
     </row>
     <row r="125" spans="1:9" ht="26.4">
-      <c r="A125" s="17">
+      <c r="A125" s="16">
         <v>124</v>
       </c>
-      <c r="B125" s="17" t="s">
+      <c r="B125" s="16" t="s">
         <v>154</v>
       </c>
       <c r="C125" s="15"/>
@@ -3270,10 +3270,10 @@
       <c r="I125" s="14"/>
     </row>
     <row r="126" spans="1:9" ht="39.6">
-      <c r="A126" s="17">
+      <c r="A126" s="16">
         <v>125</v>
       </c>
-      <c r="B126" s="17" t="s">
+      <c r="B126" s="16" t="s">
         <v>155</v>
       </c>
       <c r="C126" s="15"/>
@@ -3285,10 +3285,10 @@
       <c r="I126" s="14"/>
     </row>
     <row r="127" spans="1:9" ht="39.6">
-      <c r="A127" s="17">
+      <c r="A127" s="16">
         <v>126</v>
       </c>
-      <c r="B127" s="17" t="s">
+      <c r="B127" s="16" t="s">
         <v>156</v>
       </c>
       <c r="C127" s="15"/>
@@ -3300,10 +3300,10 @@
       <c r="I127" s="14"/>
     </row>
     <row r="128" spans="1:9" ht="26.4">
-      <c r="A128" s="17">
+      <c r="A128" s="16">
         <v>127</v>
       </c>
-      <c r="B128" s="17" t="s">
+      <c r="B128" s="16" t="s">
         <v>157</v>
       </c>
       <c r="C128" s="15"/>
@@ -3315,10 +3315,10 @@
       <c r="I128" s="14"/>
     </row>
     <row r="129" spans="1:9" ht="26.4">
-      <c r="A129" s="17">
+      <c r="A129" s="16">
         <v>128</v>
       </c>
-      <c r="B129" s="17" t="s">
+      <c r="B129" s="16" t="s">
         <v>158</v>
       </c>
       <c r="C129" s="15"/>
@@ -3330,10 +3330,10 @@
       <c r="I129" s="14"/>
     </row>
     <row r="130" spans="1:9" ht="39.6">
-      <c r="A130" s="17">
+      <c r="A130" s="16">
         <v>129</v>
       </c>
-      <c r="B130" s="17" t="s">
+      <c r="B130" s="16" t="s">
         <v>159</v>
       </c>
       <c r="C130" s="15"/>
@@ -3345,10 +3345,10 @@
       <c r="I130" s="14"/>
     </row>
     <row r="131" spans="1:9" ht="39.6">
-      <c r="A131" s="17">
+      <c r="A131" s="16">
         <v>130</v>
       </c>
-      <c r="B131" s="17" t="s">
+      <c r="B131" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C131" s="15"/>
@@ -3360,10 +3360,10 @@
       <c r="I131" s="14"/>
     </row>
     <row r="132" spans="1:9" ht="26.4">
-      <c r="A132" s="17">
+      <c r="A132" s="16">
         <v>131</v>
       </c>
-      <c r="B132" s="17" t="s">
+      <c r="B132" s="16" t="s">
         <v>161</v>
       </c>
       <c r="C132" s="15"/>
@@ -3375,10 +3375,10 @@
       <c r="I132" s="14"/>
     </row>
     <row r="133" spans="1:9" ht="26.4">
-      <c r="A133" s="17">
+      <c r="A133" s="16">
         <v>132</v>
       </c>
-      <c r="B133" s="17" t="s">
+      <c r="B133" s="16" t="s">
         <v>162</v>
       </c>
       <c r="C133" s="15"/>
@@ -3390,10 +3390,10 @@
       <c r="I133" s="14"/>
     </row>
     <row r="134" spans="1:9" ht="39.6">
-      <c r="A134" s="17">
+      <c r="A134" s="16">
         <v>133</v>
       </c>
-      <c r="B134" s="17" t="s">
+      <c r="B134" s="16" t="s">
         <v>163</v>
       </c>
       <c r="C134" s="15"/>
@@ -3405,10 +3405,10 @@
       <c r="I134" s="14"/>
     </row>
     <row r="135" spans="1:9" ht="39.6">
-      <c r="A135" s="17">
+      <c r="A135" s="16">
         <v>134</v>
       </c>
-      <c r="B135" s="17" t="s">
+      <c r="B135" s="16" t="s">
         <v>164</v>
       </c>
       <c r="C135" s="15"/>
@@ -3420,10 +3420,10 @@
       <c r="I135" s="14"/>
     </row>
     <row r="136" spans="1:9" ht="39.6">
-      <c r="A136" s="17">
+      <c r="A136" s="16">
         <v>135</v>
       </c>
-      <c r="B136" s="17" t="s">
+      <c r="B136" s="16" t="s">
         <v>165</v>
       </c>
       <c r="C136" s="15"/>
@@ -3435,7 +3435,7 @@
       <c r="I136" s="14"/>
     </row>
     <row r="137" spans="1:9" ht="39.6">
-      <c r="A137" s="17">
+      <c r="A137" s="16">
         <v>136</v>
       </c>
       <c r="B137" s="11" t="s">
@@ -3450,10 +3450,10 @@
       <c r="I137" s="14"/>
     </row>
     <row r="138" spans="1:9" ht="39.6">
-      <c r="A138" s="17">
+      <c r="A138" s="16">
         <v>137</v>
       </c>
-      <c r="B138" s="17" t="s">
+      <c r="B138" s="16" t="s">
         <v>167</v>
       </c>
       <c r="C138" s="15"/>
@@ -3465,122 +3465,122 @@
       <c r="I138" s="14"/>
     </row>
     <row r="139" spans="1:9" ht="26.4">
-      <c r="A139" s="17">
+      <c r="A139" s="16">
         <v>138</v>
       </c>
-      <c r="B139" s="17" t="s">
+      <c r="B139" s="16" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="140" spans="1:9" ht="26.4">
-      <c r="A140" s="17">
+      <c r="A140" s="16">
         <v>139</v>
       </c>
-      <c r="B140" s="17" t="s">
+      <c r="B140" s="16" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="141" spans="1:9">
-      <c r="A141" s="17">
+      <c r="A141" s="16">
         <v>140</v>
       </c>
-      <c r="B141" s="17" t="s">
+      <c r="B141" s="16" t="s">
         <v>170</v>
       </c>
     </row>
     <row r="142" spans="1:9" ht="26.4">
-      <c r="A142" s="17">
+      <c r="A142" s="16">
         <v>141</v>
       </c>
-      <c r="B142" s="17" t="s">
+      <c r="B142" s="16" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="143" spans="1:9" ht="26.4">
-      <c r="A143" s="17">
+      <c r="A143" s="16">
         <v>142</v>
       </c>
-      <c r="B143" s="17" t="s">
+      <c r="B143" s="16" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="144" spans="1:9">
-      <c r="A144" s="17">
+      <c r="A144" s="16">
         <v>143</v>
       </c>
-      <c r="B144" s="17" t="s">
+      <c r="B144" s="16" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="145" spans="1:2" ht="26.4">
-      <c r="A145" s="17">
+      <c r="A145" s="16">
         <v>144</v>
       </c>
-      <c r="B145" s="17" t="s">
+      <c r="B145" s="16" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="146" spans="1:2" ht="26.4">
-      <c r="A146" s="17">
+      <c r="A146" s="16">
         <v>145</v>
       </c>
-      <c r="B146" s="17" t="s">
+      <c r="B146" s="16" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="39.6">
-      <c r="A147" s="17">
+      <c r="A147" s="16">
         <v>146</v>
       </c>
-      <c r="B147" s="17" t="s">
+      <c r="B147" s="16" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="148" spans="1:2" ht="39.6">
-      <c r="A148" s="17">
+      <c r="A148" s="16">
         <v>147</v>
       </c>
-      <c r="B148" s="17" t="s">
+      <c r="B148" s="16" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="149" spans="1:2" ht="26.4">
-      <c r="A149" s="17">
+      <c r="A149" s="16">
         <v>148</v>
       </c>
-      <c r="B149" s="17" t="s">
+      <c r="B149" s="16" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="150" spans="1:2" ht="39.6">
-      <c r="A150" s="17">
+      <c r="A150" s="16">
         <v>149</v>
       </c>
-      <c r="B150" s="17" t="s">
+      <c r="B150" s="16" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="151" spans="1:2" ht="26.4">
-      <c r="A151" s="17">
+      <c r="A151" s="16">
         <v>150</v>
       </c>
-      <c r="B151" s="17" t="s">
+      <c r="B151" s="16" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="39.6">
-      <c r="A152" s="17">
+      <c r="A152" s="16">
         <v>151</v>
       </c>
-      <c r="B152" s="17" t="s">
+      <c r="B152" s="16" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="153" spans="1:2" ht="26.4">
-      <c r="A153" s="17">
+      <c r="A153" s="16">
         <v>152</v>
       </c>
-      <c r="B153" s="17" t="s">
+      <c r="B153" s="16" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3588,7 +3588,7 @@
       <c r="A154" s="11">
         <v>153</v>
       </c>
-      <c r="B154" s="17" t="s">
+      <c r="B154" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3596,7 +3596,7 @@
       <c r="A155" s="11">
         <v>154</v>
       </c>
-      <c r="B155" s="17" t="s">
+      <c r="B155" s="16" t="s">
         <v>16</v>
       </c>
     </row>
@@ -3604,7 +3604,7 @@
       <c r="A156" s="11">
         <v>155</v>
       </c>
-      <c r="B156" s="17" t="s">
+      <c r="B156" s="16" t="s">
         <v>17</v>
       </c>
     </row>
@@ -3612,7 +3612,7 @@
       <c r="A157" s="11">
         <v>156</v>
       </c>
-      <c r="B157" s="17" t="s">
+      <c r="B157" s="16" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3620,7 +3620,7 @@
       <c r="A158" s="11">
         <v>157</v>
       </c>
-      <c r="B158" s="17" t="s">
+      <c r="B158" s="16" t="s">
         <v>19</v>
       </c>
     </row>
@@ -3628,7 +3628,7 @@
       <c r="A159" s="11">
         <v>158</v>
       </c>
-      <c r="B159" s="17" t="s">
+      <c r="B159" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
       <c r="A160" s="11">
         <v>159</v>
       </c>
-      <c r="B160" s="17" t="s">
+      <c r="B160" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -3644,7 +3644,7 @@
       <c r="A161" s="11">
         <v>160</v>
       </c>
-      <c r="B161" s="17" t="s">
+      <c r="B161" s="16" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3652,7 +3652,7 @@
       <c r="A162" s="11">
         <v>161</v>
       </c>
-      <c r="B162" s="17" t="s">
+      <c r="B162" s="16" t="s">
         <v>23</v>
       </c>
     </row>
@@ -3660,7 +3660,7 @@
       <c r="A163" s="11">
         <v>162</v>
       </c>
-      <c r="B163" s="17" t="s">
+      <c r="B163" s="16" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>